<commit_message>
Cambios en la interfaz 3
Cambios en la interfaz 3
</commit_message>
<xml_diff>
--- a/data/Ejemplo.xlsx
+++ b/data/Ejemplo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Univerdidad UTPL\Documentos\Noveno Ciclo\Proyecto de fin de carrera 4.1\Proyecto\ADF\Pruebas_Funciones\Interfaz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SIEC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="205">
   <si>
     <t>Atributo</t>
   </si>
@@ -41,9 +41,6 @@
     <t xml:space="preserve">Pendiente </t>
   </si>
   <si>
-    <t xml:space="preserve">≥ 0% a &lt;4% </t>
-  </si>
-  <si>
     <t>Adecuada</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t xml:space="preserve">Realineamiento horizontal </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t xml:space="preserve">5 a &lt;10 m </t>
   </si>
   <si>
-    <t xml:space="preserve">Ancho del carril </t>
-  </si>
-  <si>
     <t xml:space="preserve">Línea central ancha </t>
   </si>
   <si>
@@ -158,18 +149,9 @@
     <t xml:space="preserve">Ampliar/Ensanchar carril (hasta 0.5 m) </t>
   </si>
   <si>
-    <t>Bandas alertadoras sobre berma/acotamiento</t>
-  </si>
-  <si>
-    <t>Eliminar peligros laterales – lado del pasajero</t>
-  </si>
-  <si>
     <t>Mejoramiento de taludes y terraplenes laterales – lado conductor</t>
   </si>
   <si>
-    <t>Mejoramiento de taludes y terraplenes laterales – lado del pasajero</t>
-  </si>
-  <si>
     <t>Pavimentado – regular</t>
   </si>
   <si>
@@ -200,9 +182,6 @@
     <t xml:space="preserve">Mejora en cruce ferroviario </t>
   </si>
   <si>
-    <t xml:space="preserve">Rotonda/Glorieta </t>
-  </si>
-  <si>
     <t xml:space="preserve">Pavimentar superficie de la vía </t>
   </si>
   <si>
@@ -287,16 +266,10 @@
     <t xml:space="preserve">Calidad de la curva </t>
   </si>
   <si>
-    <t>Camates del tráfico</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mejoras de estacionamiento </t>
   </si>
   <si>
     <t>Barreras laterales (carril para bicicletas)</t>
-  </si>
-  <si>
-    <t>Acera peatonal de lado del pasajero (adyacente al camino)</t>
   </si>
   <si>
     <t>Provisión de acera costado del conductor (con barrera)</t>
@@ -410,24 +383,9 @@
     <t xml:space="preserve">Ampliar/Ensanchar carril (&gt; 0.5 m) </t>
   </si>
   <si>
-    <t xml:space="preserve">Pavimentación de berma/acotamiento de lado del copiloto mayor a 1 m. </t>
-  </si>
-  <si>
-    <t>Pavimentación de berma/acotamiento de lado del copiloto hasta 1 m.</t>
-  </si>
-  <si>
-    <t>Acera peatonal de lado del pasajero (separada del camino &gt; 3 m)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Provisión de sendero peatonal informal &gt; 1m del lado del copiloto </t>
   </si>
   <si>
-    <t>Pavimentación de berma/acotamiento del lado del conductor mayor a 1 m.</t>
-  </si>
-  <si>
-    <t>Pavimentación de berma/acotamiento del lado del conductor hasta 1 m</t>
-  </si>
-  <si>
     <t>Distancia de visibilidad</t>
   </si>
   <si>
@@ -527,9 +485,6 @@
     <t>5 a &lt; 10 m</t>
   </si>
   <si>
-    <t>Barrera de seguridad: amigable para motocicletas</t>
-  </si>
-  <si>
     <t>≥ 10 m</t>
   </si>
   <si>
@@ -654,6 +609,48 @@
   </si>
   <si>
     <t>Velocidad de operación (percentil 85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ancho de carril </t>
+  </si>
+  <si>
+    <t>Barrera de seguridad - amigable para motocicletas</t>
+  </si>
+  <si>
+    <t>Infraestructura de cruce peatonal en la intersección</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pavimentación de espaldón de lado del copiloto mayor a 1 m. </t>
+  </si>
+  <si>
+    <t>Pavimentación de espaldón de lado del copiloto hasta 1 m.</t>
+  </si>
+  <si>
+    <t>Bandas alertadoras sobre el espaldón</t>
+  </si>
+  <si>
+    <t>Eliminar peligros laterales – lado del copiloto</t>
+  </si>
+  <si>
+    <t>Mejoramiento de taludes y terraplenes laterales – lado del copiloto</t>
+  </si>
+  <si>
+    <t>Acera peatonal de lado del copiloto (separada del camino &gt; 3 m)</t>
+  </si>
+  <si>
+    <t>Acera peatonal de lado del copiloto (adyacente al camino)</t>
+  </si>
+  <si>
+    <t>Calmates del tráfico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">≥ 0 % a &lt; 4 % </t>
+  </si>
+  <si>
+    <t>Pavimentación de espaldón de lado del conductor mayor a 1 m.</t>
+  </si>
+  <si>
+    <t>Pavimentación de espaldón de lado del conductor hasta 1 m</t>
   </si>
 </sst>
 </file>
@@ -995,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,10 +1007,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1036,7 +1033,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>202</v>
       </c>
       <c r="E2" s="1" t="b">
         <f>FALSE</f>
@@ -1048,13 +1045,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="b">
         <f>FALSE</f>
@@ -1066,13 +1063,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E4" s="1" t="b">
         <f>FALSE</f>
@@ -1084,25 +1081,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="E5" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="1" t="b">
         <f>FALSE</f>
@@ -1114,28 +1117,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E7" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="b">
         <f>FALSE</f>
@@ -1147,28 +1153,31 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E9" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1" t="b">
         <f>FALSE</f>
@@ -1180,25 +1189,31 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E11" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1" t="b">
         <f>FALSE</f>
@@ -1210,55 +1225,67 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E13" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E15" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1" t="b">
         <f>FALSE</f>
@@ -1270,13 +1297,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E17" s="1" t="b">
         <f>FALSE</f>
@@ -1284,11 +1311,17 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1" t="b">
         <f>FALSE</f>
@@ -1300,13 +1333,13 @@
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" s="1" t="b">
         <f>FALSE</f>
@@ -1314,11 +1347,17 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E20" s="1" t="b">
         <f>FALSE</f>
@@ -1330,13 +1369,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E21" s="1" t="b">
         <f>FALSE</f>
@@ -1348,13 +1387,13 @@
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E22" s="1" t="b">
         <f>FALSE</f>
@@ -1366,13 +1405,13 @@
         <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E23" s="1" t="b">
         <f>FALSE</f>
@@ -1384,13 +1423,13 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E24" s="1" t="b">
         <f>FALSE</f>
@@ -1402,13 +1441,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E25" s="1" t="b">
         <f>FALSE</f>
@@ -1420,13 +1459,13 @@
         <v>17</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E26" s="1" t="b">
         <f>FALSE</f>
@@ -1438,31 +1477,31 @@
         <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="E27" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E28" s="1" t="b">
         <f>FALSE</f>
@@ -1474,13 +1513,13 @@
         <v>20</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E29" s="1" t="b">
         <f>FALSE</f>
@@ -1492,13 +1531,13 @@
         <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="E30" s="1" t="b">
         <f>FALSE</f>
@@ -1510,13 +1549,13 @@
         <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="E31" s="1" t="b">
         <f>FALSE</f>
@@ -1528,13 +1567,13 @@
         <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="E32" s="1" t="b">
         <f>FALSE</f>
@@ -1546,13 +1585,13 @@
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E33" s="1" t="b">
         <f>FALSE</f>
@@ -1564,13 +1603,13 @@
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E34" s="1" t="b">
         <f>FALSE</f>
@@ -1582,13 +1621,13 @@
         <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E35" s="1" t="b">
         <f>FALSE</f>
@@ -1600,13 +1639,13 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="E36" s="1" t="b">
         <f>FALSE</f>
@@ -1618,13 +1657,13 @@
         <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>128</v>
+        <v>203</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E37" s="1" t="b">
         <f>FALSE</f>
@@ -1636,13 +1675,13 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>129</v>
+        <v>204</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="E38" s="1" t="b">
         <f>FALSE</f>
@@ -1654,13 +1693,13 @@
         <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E39" s="1" t="b">
         <f>FALSE</f>
@@ -1672,13 +1711,13 @@
         <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E40" s="1" t="b">
         <f>FALSE</f>
@@ -1686,11 +1725,17 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>31</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C41" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="E41" s="1" t="b">
         <f>FALSE</f>
@@ -1702,13 +1747,13 @@
         <v>32</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E42" s="1" t="b">
         <f>FALSE</f>
@@ -1716,11 +1761,17 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>32</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C43" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="E43" s="1" t="b">
         <f>FALSE</f>
@@ -1732,13 +1783,13 @@
         <v>33</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E44" s="1" t="b">
         <f>FALSE</f>
@@ -1746,11 +1797,17 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>33</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="C45" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E45" s="1" t="b">
         <f>FALSE</f>
@@ -1762,13 +1819,13 @@
         <v>34</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>45</v>
+        <v>197</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E46" s="1" t="b">
         <f>FALSE</f>
@@ -1776,11 +1833,17 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>34</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="C47" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E47" s="1" t="b">
         <f>FALSE</f>
@@ -1792,13 +1855,13 @@
         <v>35</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E48" s="1" t="b">
         <f>FALSE</f>
@@ -1806,11 +1869,17 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>35</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C49" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E49" s="1" t="b">
         <f>FALSE</f>
@@ -1822,13 +1891,13 @@
         <v>36</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>47</v>
+        <v>198</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E50" s="1" t="b">
         <f>FALSE</f>
@@ -1836,11 +1905,17 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>36</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="C51" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E51" s="1" t="b">
         <f>FALSE</f>
@@ -1852,13 +1927,13 @@
         <v>37</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="E52" s="1" t="b">
         <f>FALSE</f>
@@ -1870,31 +1945,31 @@
         <v>38</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E53" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>39</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E54" s="1" t="b">
         <f>FALSE</f>
@@ -1906,13 +1981,13 @@
         <v>40</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E55" s="1" t="b">
         <f>FALSE</f>
@@ -1924,13 +1999,13 @@
         <v>41</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="E56" s="1" t="b">
         <f>FALSE</f>
@@ -1942,13 +2017,13 @@
         <v>42</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E57" s="1" t="b">
         <f>FALSE</f>
@@ -1960,13 +2035,13 @@
         <v>43</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E58" s="1" t="b">
         <f>FALSE</f>
@@ -1978,13 +2053,13 @@
         <v>44</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E59" s="1" t="b">
         <f>FALSE</f>
@@ -1996,13 +2071,13 @@
         <v>45</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="E60" s="1" t="b">
         <f>FALSE</f>
@@ -2014,13 +2089,13 @@
         <v>46</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="E61" s="1" t="b">
         <f>FALSE</f>
@@ -2032,13 +2107,13 @@
         <v>47</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E62" s="1" t="b">
         <f>FALSE</f>
@@ -2050,13 +2125,13 @@
         <v>48</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E63" s="1" t="b">
         <f>FALSE</f>
@@ -2068,13 +2143,13 @@
         <v>49</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E64" s="1" t="b">
         <f>FALSE</f>
@@ -2082,11 +2157,17 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>49</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C65" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E65" s="1" t="b">
         <f>FALSE</f>
@@ -2098,13 +2179,13 @@
         <v>50</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="E66" s="1" t="b">
         <f>FALSE</f>
@@ -2116,13 +2197,13 @@
         <v>51</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="E67" s="1" t="b">
         <f>FALSE</f>
@@ -2134,13 +2215,13 @@
         <v>52</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E68" s="1" t="b">
         <f>FALSE</f>
@@ -2152,13 +2233,13 @@
         <v>53</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E69" s="1" t="b">
         <f>FALSE</f>
@@ -2170,13 +2251,13 @@
         <v>54</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E70" s="1" t="b">
         <f>FALSE</f>
@@ -2188,13 +2269,13 @@
         <v>55</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="E71" s="1" t="b">
         <f>FALSE</f>
@@ -2206,13 +2287,13 @@
         <v>56</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E72" s="1" t="b">
         <f>FALSE</f>
@@ -2224,13 +2305,13 @@
         <v>57</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="E73" s="1" t="b">
         <f>FALSE</f>
@@ -2242,49 +2323,49 @@
         <v>58</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="E74" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>59</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="E75" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>60</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E76" s="1" t="b">
         <f>FALSE</f>
@@ -2296,13 +2377,13 @@
         <v>61</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="E77" s="1" t="b">
         <f>FALSE</f>
@@ -2314,13 +2395,13 @@
         <v>62</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E78" s="1" t="b">
         <f>FALSE</f>
@@ -2332,13 +2413,13 @@
         <v>63</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>126</v>
+        <v>199</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="E79" s="1" t="b">
         <f>FALSE</f>
@@ -2350,13 +2431,13 @@
         <v>64</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E80" s="1" t="b">
         <f>FALSE</f>
@@ -2368,13 +2449,13 @@
         <v>65</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E81" s="1" t="b">
         <f>FALSE</f>
@@ -2386,13 +2467,13 @@
         <v>66</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E82" s="1" t="b">
         <f>FALSE</f>
@@ -2404,13 +2485,13 @@
         <v>67</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="E83" s="1" t="b">
         <f>FALSE</f>
@@ -2422,13 +2503,13 @@
         <v>68</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E84" s="1" t="b">
         <f>FALSE</f>
@@ -2440,13 +2521,13 @@
         <v>69</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E85" s="1" t="b">
         <f>FALSE</f>
@@ -2458,13 +2539,13 @@
         <v>70</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E86" s="1" t="b">
         <f>FALSE</f>
@@ -2476,13 +2557,13 @@
         <v>71</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E87" s="1" t="b">
         <f>FALSE</f>
@@ -2494,13 +2575,13 @@
         <v>72</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E88" s="1" t="b">
         <f>FALSE</f>
@@ -2512,13 +2593,13 @@
         <v>73</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E89" s="1" t="b">
         <f>FALSE</f>
@@ -2530,13 +2611,13 @@
         <v>74</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E90" s="1" t="b">
         <f>FALSE</f>
@@ -2548,13 +2629,13 @@
         <v>75</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="E91" s="1" t="b">
         <f>FALSE</f>
@@ -2566,13 +2647,13 @@
         <v>76</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="E92" s="1" t="b">
         <f>FALSE</f>
@@ -2584,13 +2665,13 @@
         <v>77</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E93" s="1" t="b">
         <f>FALSE</f>
@@ -2602,13 +2683,13 @@
         <v>78</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E94" s="1" t="b">
         <f>FALSE</f>
@@ -2620,13 +2701,13 @@
         <v>79</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E95" s="1" t="b">
         <f>FALSE</f>
@@ -2638,13 +2719,13 @@
         <v>80</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E96" s="1" t="b">
         <f>FALSE</f>
@@ -2656,13 +2737,13 @@
         <v>81</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>87</v>
+        <v>201</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E97" s="1" t="b">
         <f>FALSE</f>
@@ -2674,13 +2755,13 @@
         <v>82</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="E98" s="1" t="b">
         <f>FALSE</f>
@@ -2692,13 +2773,13 @@
         <v>83</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E99" s="1" t="b">
         <f>FALSE</f>
@@ -2706,11 +2787,17 @@
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>83</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="C100" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E100" s="1" t="b">
         <f>FALSE</f>
@@ -2722,13 +2809,13 @@
         <v>84</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E101" s="1" t="b">
         <f>FALSE</f>
@@ -2736,11 +2823,17 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>84</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="C102" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E102" s="1" t="b">
         <f>FALSE</f>
@@ -2752,13 +2845,13 @@
         <v>85</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E103" s="1" t="b">
         <f>FALSE</f>
@@ -2766,11 +2859,17 @@
       </c>
     </row>
     <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>85</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="C104" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="E104" s="1" t="b">
         <f>FALSE</f>
@@ -2782,13 +2881,13 @@
         <v>86</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="E105" s="1" t="b">
         <f>FALSE</f>
@@ -2800,25 +2899,31 @@
         <v>87</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E106" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>87</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="C107" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E107" s="1" t="b">
         <f>FALSE</f>
@@ -2830,13 +2935,13 @@
         <v>88</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E108" s="1" t="b">
         <f>FALSE</f>
@@ -2844,11 +2949,17 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>88</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C109" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E109" s="1" t="b">
         <f>FALSE</f>
@@ -2860,25 +2971,31 @@
         <v>89</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E110" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>89</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="C111" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="E111" s="1" t="b">
         <f>FALSE</f>
@@ -2890,25 +3007,31 @@
         <v>90</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E112" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>90</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="C113" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E113" s="1" t="b">
         <f>FALSE</f>
@@ -2920,25 +3043,31 @@
         <v>91</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E114" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>91</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="C115" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E115" s="1" t="b">
         <f>FALSE</f>
@@ -2950,13 +3079,13 @@
         <v>92</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E116" s="1" t="b">
         <f>FALSE</f>
@@ -2964,11 +3093,17 @@
       </c>
     </row>
     <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>92</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="C117" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="E117" s="1" t="b">
         <f>FALSE</f>
@@ -2980,13 +3115,13 @@
         <v>93</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="E118" s="1" t="b">
         <f>FALSE</f>
@@ -2998,13 +3133,13 @@
         <v>94</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="E119" s="1" t="b">
         <f>FALSE</f>

</xml_diff>

<commit_message>
Cambios realizados en la interfaz 3
Cambios en la interfaz 3
</commit_message>
<xml_diff>
--- a/data/Ejemplo.xlsx
+++ b/data/Ejemplo.xlsx
@@ -368,9 +368,6 @@
     <t>Amplicación/Duplicación de calzada con una mediana o faja separadora mayor a 20 m de ancho</t>
   </si>
   <si>
-    <t>Ampliación/Duplicación de calzada con una mediana o faja separadora de 10 a 20m dancho</t>
-  </si>
-  <si>
     <t>Ampliación/Duplicación de calzada con una mediana o faja separadora de 5 a 10 m de ancho</t>
   </si>
   <si>
@@ -641,9 +638,6 @@
     <t>Acera peatonal de lado del copiloto (adyacente al camino)</t>
   </si>
   <si>
-    <t>Calmates del tráfico</t>
-  </si>
-  <si>
     <t xml:space="preserve">≥ 0 % a &lt; 4 % </t>
   </si>
   <si>
@@ -651,6 +645,12 @@
   </si>
   <si>
     <t>Pavimentación de espaldón de lado del conductor hasta 1 m</t>
+  </si>
+  <si>
+    <t>Calmantes del tráfico</t>
+  </si>
+  <si>
+    <t>Ampliación/Duplicación de calzada con una mediana o faja separadora de 10 a 20m de ancho</t>
   </si>
 </sst>
 </file>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1033,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E2" s="1" t="b">
         <f>FALSE</f>
@@ -1048,7 +1048,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
@@ -1069,7 +1069,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" s="1" t="b">
         <f>FALSE</f>
@@ -1084,10 +1084,10 @@
         <v>109</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="E5" s="1" t="b">
         <f>FALSE</f>
@@ -1117,13 +1117,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>110</v>
+        <v>204</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E7" s="1" t="b">
         <f>FALSE</f>
@@ -1135,7 +1135,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>204</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
@@ -1153,13 +1153,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E9" s="1" t="b">
         <f>FALSE</f>
@@ -1171,7 +1171,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -1189,13 +1189,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E11" s="1" t="b">
         <f>FALSE</f>
@@ -1207,7 +1207,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>11</v>
@@ -1225,13 +1225,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" s="1" t="b">
         <f>FALSE</f>
@@ -1243,7 +1243,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
@@ -1264,10 +1264,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E15" s="1" t="b">
         <f>FALSE</f>
@@ -1300,10 +1300,10 @@
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="E17" s="1" t="b">
         <f>FALSE</f>
@@ -1318,7 +1318,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -1336,7 +1336,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -1357,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E20" s="1" t="b">
         <f>FALSE</f>
@@ -1372,10 +1372,10 @@
         <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E21" s="1" t="b">
         <f>FALSE</f>
@@ -1393,7 +1393,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E22" s="1" t="b">
         <f>FALSE</f>
@@ -1411,7 +1411,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E23" s="1" t="b">
         <f>FALSE</f>
@@ -1426,7 +1426,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>18</v>
@@ -1444,10 +1444,10 @@
         <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E25" s="1" t="b">
         <f>FALSE</f>
@@ -1462,7 +1462,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>18</v>
@@ -1480,10 +1480,10 @@
         <v>29</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E27" s="1" t="b">
         <f>FALSE</f>
@@ -1498,10 +1498,10 @@
         <v>37</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E28" s="1" t="b">
         <f>FALSE</f>
@@ -1516,10 +1516,10 @@
         <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E29" s="1" t="b">
         <f>FALSE</f>
@@ -1534,10 +1534,10 @@
         <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="E30" s="1" t="b">
         <f>FALSE</f>
@@ -1552,10 +1552,10 @@
         <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E31" s="1" t="b">
         <f>FALSE</f>
@@ -1570,10 +1570,10 @@
         <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E32" s="1" t="b">
         <f>FALSE</f>
@@ -1585,13 +1585,13 @@
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E33" s="1" t="b">
         <f>FALSE</f>
@@ -1606,10 +1606,10 @@
         <v>40</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E34" s="1" t="b">
         <f>FALSE</f>
@@ -1621,13 +1621,13 @@
         <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E35" s="1" t="b">
         <f>FALSE</f>
@@ -1639,13 +1639,13 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E36" s="1" t="b">
         <f>FALSE</f>
@@ -1657,13 +1657,13 @@
         <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E37" s="1" t="b">
         <f>FALSE</f>
@@ -1675,13 +1675,13 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38" s="1" t="b">
         <f>FALSE</f>
@@ -1693,10 +1693,10 @@
         <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>30</v>
@@ -1714,10 +1714,10 @@
         <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E40" s="1" t="b">
         <f>FALSE</f>
@@ -1732,10 +1732,10 @@
         <v>34</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E41" s="1" t="b">
         <f>FALSE</f>
@@ -1750,7 +1750,7 @@
         <v>35</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>31</v>
@@ -1768,10 +1768,10 @@
         <v>35</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E43" s="1" t="b">
         <f>FALSE</f>
@@ -1786,10 +1786,10 @@
         <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E44" s="1" t="b">
         <f>FALSE</f>
@@ -1804,10 +1804,10 @@
         <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E45" s="1" t="b">
         <f>FALSE</f>
@@ -1819,13 +1819,13 @@
         <v>34</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E46" s="1" t="b">
         <f>FALSE</f>
@@ -1837,13 +1837,13 @@
         <v>34</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E47" s="1" t="b">
         <f>FALSE</f>
@@ -1858,10 +1858,10 @@
         <v>41</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E48" s="1" t="b">
         <f>FALSE</f>
@@ -1876,10 +1876,10 @@
         <v>41</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E49" s="1" t="b">
         <f>FALSE</f>
@@ -1891,13 +1891,13 @@
         <v>36</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E50" s="1" t="b">
         <f>FALSE</f>
@@ -1909,13 +1909,13 @@
         <v>36</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E51" s="1" t="b">
         <f>FALSE</f>
@@ -1927,13 +1927,13 @@
         <v>37</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E52" s="1" t="b">
         <f>FALSE</f>
@@ -1948,7 +1948,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>42</v>
@@ -1966,7 +1966,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>43</v>
@@ -1984,10 +1984,10 @@
         <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E55" s="1" t="b">
         <f>FALSE</f>
@@ -2002,10 +2002,10 @@
         <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E56" s="1" t="b">
         <f>FALSE</f>
@@ -2023,7 +2023,7 @@
         <v>26</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E57" s="1" t="b">
         <f>FALSE</f>
@@ -2041,7 +2041,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E58" s="1" t="b">
         <f>FALSE</f>
@@ -2059,7 +2059,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E59" s="1" t="b">
         <f>FALSE</f>
@@ -2077,7 +2077,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E60" s="1" t="b">
         <f>FALSE</f>
@@ -2095,7 +2095,7 @@
         <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E61" s="1" t="b">
         <f>FALSE</f>
@@ -2113,7 +2113,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E62" s="1" t="b">
         <f>FALSE</f>
@@ -2131,7 +2131,7 @@
         <v>46</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E63" s="1" t="b">
         <f>FALSE</f>
@@ -2182,10 +2182,10 @@
         <v>61</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="E66" s="1" t="b">
         <f>FALSE</f>
@@ -2200,10 +2200,10 @@
         <v>62</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E67" s="1" t="b">
         <f>FALSE</f>
@@ -2218,10 +2218,10 @@
         <v>63</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="E68" s="1" t="b">
         <f>FALSE</f>
@@ -2236,10 +2236,10 @@
         <v>64</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E69" s="1" t="b">
         <f>FALSE</f>
@@ -2254,10 +2254,10 @@
         <v>65</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E70" s="1" t="b">
         <f>FALSE</f>
@@ -2272,10 +2272,10 @@
         <v>66</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E71" s="1" t="b">
         <f>FALSE</f>
@@ -2290,10 +2290,10 @@
         <v>67</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E72" s="1" t="b">
         <f>FALSE</f>
@@ -2308,10 +2308,10 @@
         <v>68</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E73" s="1" t="b">
         <f>FALSE</f>
@@ -2326,10 +2326,10 @@
         <v>69</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="E74" s="1" t="b">
         <f>FALSE</f>
@@ -2344,10 +2344,10 @@
         <v>70</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E75" s="1" t="b">
         <f>FALSE</f>
@@ -2362,10 +2362,10 @@
         <v>71</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E76" s="1" t="b">
         <f>FALSE</f>
@@ -2380,10 +2380,10 @@
         <v>72</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E77" s="1" t="b">
         <f>FALSE</f>
@@ -2398,10 +2398,10 @@
         <v>73</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E78" s="1" t="b">
         <f>FALSE</f>
@@ -2413,13 +2413,13 @@
         <v>63</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E79" s="1" t="b">
         <f>FALSE</f>
@@ -2431,13 +2431,13 @@
         <v>64</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E80" s="1" t="b">
         <f>FALSE</f>
@@ -2449,13 +2449,13 @@
         <v>65</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E81" s="1" t="b">
         <f>FALSE</f>
@@ -2470,7 +2470,7 @@
         <v>82</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>45</v>
@@ -2488,10 +2488,10 @@
         <v>83</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E83" s="1" t="b">
         <f>FALSE</f>
@@ -2506,10 +2506,10 @@
         <v>84</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E84" s="1" t="b">
         <f>FALSE</f>
@@ -2524,10 +2524,10 @@
         <v>85</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E85" s="1" t="b">
         <f>FALSE</f>
@@ -2614,7 +2614,7 @@
         <v>90</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>12</v>
@@ -2632,10 +2632,10 @@
         <v>91</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="E91" s="1" t="b">
         <f>FALSE</f>
@@ -2650,10 +2650,10 @@
         <v>92</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E92" s="1" t="b">
         <f>FALSE</f>
@@ -2704,7 +2704,7 @@
         <v>95</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>5</v>
@@ -2722,7 +2722,7 @@
         <v>96</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>74</v>
@@ -2737,10 +2737,10 @@
         <v>81</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>30</v>
@@ -2761,7 +2761,7 @@
         <v>75</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E98" s="1" t="b">
         <f>FALSE</f>
@@ -2776,10 +2776,10 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E99" s="1" t="b">
         <f>FALSE</f>
@@ -2794,10 +2794,10 @@
         <v>97</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E100" s="1" t="b">
         <f>FALSE</f>
@@ -2812,10 +2812,10 @@
         <v>98</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E101" s="1" t="b">
         <f>FALSE</f>
@@ -2830,10 +2830,10 @@
         <v>98</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E102" s="1" t="b">
         <f>FALSE</f>
@@ -2848,10 +2848,10 @@
         <v>81</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E103" s="1" t="b">
         <f>FALSE</f>
@@ -2866,10 +2866,10 @@
         <v>81</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E104" s="1" t="b">
         <f>FALSE</f>
@@ -2884,10 +2884,10 @@
         <v>99</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E105" s="1" t="b">
         <f>FALSE</f>
@@ -2902,10 +2902,10 @@
         <v>101</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E106" s="1" t="b">
         <f>FALSE</f>
@@ -2920,10 +2920,10 @@
         <v>101</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E107" s="1" t="b">
         <f>FALSE</f>
@@ -2938,10 +2938,10 @@
         <v>102</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E108" s="1" t="b">
         <f>FALSE</f>
@@ -2956,10 +2956,10 @@
         <v>102</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E109" s="1" t="b">
         <f>FALSE</f>
@@ -2974,10 +2974,10 @@
         <v>103</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E110" s="1" t="b">
         <f>FALSE</f>
@@ -2992,10 +2992,10 @@
         <v>103</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E111" s="1" t="b">
         <f>FALSE</f>
@@ -3010,10 +3010,10 @@
         <v>104</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E112" s="1" t="b">
         <f>FALSE</f>
@@ -3028,10 +3028,10 @@
         <v>104</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E113" s="1" t="b">
         <f>FALSE</f>
@@ -3046,10 +3046,10 @@
         <v>105</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E114" s="1" t="b">
         <f>FALSE</f>
@@ -3064,10 +3064,10 @@
         <v>105</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E115" s="1" t="b">
         <f>FALSE</f>
@@ -3082,10 +3082,10 @@
         <v>106</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E116" s="1" t="b">
         <f>FALSE</f>
@@ -3100,10 +3100,10 @@
         <v>106</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E117" s="1" t="b">
         <f>FALSE</f>
@@ -3118,10 +3118,10 @@
         <v>107</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E118" s="1" t="b">
         <f>FALSE</f>
@@ -3139,7 +3139,7 @@
         <v>100</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E119" s="1" t="b">
         <f>FALSE</f>

</xml_diff>